<commit_message>
Update Height and Weight lower boud
Lower bound of height changed to 120 cm and weight to 35 kg
</commit_message>
<xml_diff>
--- a/BCRPP_QC_R_Excel_Program/BCRPP_QC_Version_1/Core QC Rules/BCRPP Warning Rules.xlsx
+++ b/BCRPP_QC_R_Excel_Program/BCRPP_QC_Version_1/Core QC Rules/BCRPP Warning Rules.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82AF73AA-04F8-5D46-AE2D-F8160668CA36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FC5E05-88D5-4EAE-B9E8-BC9DD845BE04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$T$110</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$T$111</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="352">
   <si>
     <t>Variable</t>
   </si>
@@ -1083,6 +1083,15 @@
   </si>
   <si>
     <t>Please provide an explanation for why lastfup is missing/unknown.</t>
+  </si>
+  <si>
+    <t>Parity</t>
+  </si>
+  <si>
+    <t>1 &lt;= Parity &amp; Parity &lt; 15 | Parity == 888</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify Parity: Parous=1, but parity less than 1 or more than 15 pregnancies  </t>
   </si>
 </sst>
 </file>
@@ -1455,38 +1464,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T113"/>
+  <dimension ref="A1:U114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B87" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="T113" sqref="T113"/>
+    <sheetView tabSelected="1" topLeftCell="G64" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88:G88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="74.6640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="16.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="28.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="97" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="24.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="119.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="255.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="64.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="180" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1548,7 +1557,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
@@ -1574,7 +1583,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
@@ -1600,7 +1609,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
@@ -1617,7 +1626,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
@@ -1637,7 +1646,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>33</v>
       </c>
@@ -1660,7 +1669,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
@@ -1686,7 +1695,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
@@ -1709,7 +1718,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>43</v>
       </c>
@@ -1726,7 +1735,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>46</v>
       </c>
@@ -1746,7 +1755,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>48</v>
       </c>
@@ -1763,7 +1772,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>51</v>
       </c>
@@ -1771,7 +1780,7 @@
         <v>34</v>
       </c>
       <c r="C12" s="2">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D12" s="2">
         <v>100</v>
@@ -1783,7 +1792,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>53</v>
       </c>
@@ -1800,7 +1809,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>56</v>
       </c>
@@ -1817,7 +1826,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>58</v>
       </c>
@@ -1834,7 +1843,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>61</v>
       </c>
@@ -1851,7 +1860,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>63</v>
       </c>
@@ -1871,7 +1880,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>64</v>
       </c>
@@ -1879,7 +1888,7 @@
         <v>34</v>
       </c>
       <c r="C18" s="2">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="D18" s="2">
         <v>200</v>
@@ -1891,7 +1900,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>66</v>
       </c>
@@ -1899,7 +1908,7 @@
         <v>34</v>
       </c>
       <c r="C19" s="2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D19" s="2">
         <v>50</v>
@@ -1911,7 +1920,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>68</v>
       </c>
@@ -1919,7 +1928,7 @@
         <v>34</v>
       </c>
       <c r="C20" s="2">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D20" s="2">
         <v>150</v>
@@ -1931,7 +1940,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>70</v>
       </c>
@@ -1939,7 +1948,7 @@
         <v>34</v>
       </c>
       <c r="C21" s="2">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D21" s="2">
         <v>50</v>
@@ -1951,7 +1960,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>72</v>
       </c>
@@ -1971,7 +1980,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>74</v>
       </c>
@@ -1991,7 +2000,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>76</v>
       </c>
@@ -2011,7 +2020,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>78</v>
       </c>
@@ -2031,7 +2040,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
         <v>80</v>
       </c>
@@ -2051,7 +2060,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
         <v>82</v>
       </c>
@@ -2071,7 +2080,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
         <v>84</v>
       </c>
@@ -2091,7 +2100,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
         <v>86</v>
       </c>
@@ -2111,7 +2120,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A30" s="2" t="s">
         <v>88</v>
       </c>
@@ -2131,7 +2140,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
         <v>90</v>
       </c>
@@ -2151,7 +2160,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
         <v>92</v>
       </c>
@@ -2171,7 +2180,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
         <v>94</v>
       </c>
@@ -2191,7 +2200,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A34" s="2" t="s">
         <v>96</v>
       </c>
@@ -2211,33 +2220,46 @@
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B35" s="2" t="s">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A35" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G35" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="S35" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="T35" s="2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="J35" s="3">
+        <v>1</v>
+      </c>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+      <c r="R35" s="3"/>
+      <c r="S35" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="T35" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="U35" s="3"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A36" s="2" t="s">
         <v>98</v>
       </c>
@@ -2245,25 +2267,25 @@
         <v>21</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>329</v>
+        <v>100</v>
       </c>
       <c r="I36" s="2" t="s">
         <v>98</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="S36" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="T36" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A37" s="2" t="s">
         <v>98</v>
       </c>
@@ -2271,25 +2293,25 @@
         <v>21</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I37" s="2" t="s">
         <v>98</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="S37" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="T37" s="2" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A38" s="2" t="s">
         <v>98</v>
       </c>
@@ -2297,25 +2319,25 @@
         <v>21</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>98</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="S38" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="T38" s="3" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="T38" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A39" s="2" t="s">
         <v>98</v>
       </c>
@@ -2323,25 +2345,25 @@
         <v>21</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>98</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S39" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="T39" s="3" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A40" s="2" t="s">
         <v>98</v>
       </c>
@@ -2349,25 +2371,25 @@
         <v>21</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>98</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="S40" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="T40" s="3" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A41" s="2" t="s">
         <v>98</v>
       </c>
@@ -2375,25 +2397,25 @@
         <v>21</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>98</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="S41" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="T41" s="3" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A42" s="2" t="s">
         <v>98</v>
       </c>
@@ -2401,25 +2423,25 @@
         <v>21</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="S42" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="T42" s="3" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A43" s="2" t="s">
         <v>98</v>
       </c>
@@ -2427,65 +2449,53 @@
         <v>21</v>
       </c>
       <c r="G43" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="S43" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="T43" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A44" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G44" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="H43" s="2" t="s">
+      <c r="H44" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="I43" s="2" t="s">
+      <c r="I44" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="J43" s="2" t="s">
+      <c r="J44" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="S43" s="2" t="s">
+      <c r="S44" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="T43" s="3" t="s">
+      <c r="T44" s="3" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A45" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C44" s="2">
-        <v>0</v>
-      </c>
-      <c r="D44" s="2">
-        <v>24</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="L44" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="M44" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="S44" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="T44" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>111</v>
@@ -2500,7 +2510,7 @@
         <v>110</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>112</v>
@@ -2512,18 +2522,18 @@
         <v>98</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="S45" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="T45" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A46" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="T45" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>111</v>
@@ -2535,10 +2545,10 @@
         <v>24</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>112</v>
@@ -2550,18 +2560,18 @@
         <v>98</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="S46" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="T46" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A47" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="T46" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>111</v>
@@ -2573,10 +2583,10 @@
         <v>24</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I47" s="2" t="s">
         <v>112</v>
@@ -2588,18 +2598,18 @@
         <v>98</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="S47" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="S47" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="T47" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A48" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="T47" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>111</v>
@@ -2611,10 +2621,10 @@
         <v>24</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I48" s="2" t="s">
         <v>112</v>
@@ -2626,18 +2636,18 @@
         <v>98</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="S48" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="T48" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A49" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="T48" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>111</v>
@@ -2649,10 +2659,10 @@
         <v>24</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I49" s="2" t="s">
         <v>112</v>
@@ -2664,18 +2674,18 @@
         <v>98</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="S49" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="T49" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A50" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="T49" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>111</v>
@@ -2687,10 +2697,10 @@
         <v>24</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>112</v>
@@ -2702,18 +2712,18 @@
         <v>98</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="S50" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="S50" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="T50" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A51" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="T50" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>111</v>
@@ -2725,10 +2735,10 @@
         <v>24</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I51" s="2" t="s">
         <v>112</v>
@@ -2740,18 +2750,18 @@
         <v>98</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="S51" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="S51" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="T51" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A52" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="T51" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>111</v>
@@ -2763,10 +2773,10 @@
         <v>24</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I52" s="2" t="s">
         <v>112</v>
@@ -2778,18 +2788,18 @@
         <v>98</v>
       </c>
       <c r="M52" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="S52" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="T52" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A53" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="T52" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>111</v>
@@ -2801,10 +2811,10 @@
         <v>24</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I53" s="2" t="s">
         <v>112</v>
@@ -2816,117 +2826,129 @@
         <v>98</v>
       </c>
       <c r="M53" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="S53" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="T53" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A54" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C54" s="2">
+        <v>0</v>
+      </c>
+      <c r="D54" s="2">
+        <v>24</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="M54" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="S53" s="2" t="s">
+      <c r="S54" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="T53" s="3" t="s">
+      <c r="T54" s="3" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="S54" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="T54" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A55" s="2" t="s">
         <v>143</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E55" s="2">
-        <v>4</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="J55" s="2">
-        <v>777</v>
-      </c>
-      <c r="L55" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="M55" s="2">
-        <v>777</v>
-      </c>
-      <c r="O55" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="P55" s="2">
-        <v>777</v>
+        <v>30</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="S55" s="2" t="s">
         <v>143</v>
       </c>
       <c r="T55" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A56" s="2" t="s">
         <v>143</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>37</v>
+        <v>146</v>
       </c>
       <c r="E56" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I56" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J56" s="2">
+        <v>777</v>
+      </c>
+      <c r="L56" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="J56" s="2">
-        <v>666</v>
+      <c r="M56" s="2">
+        <v>777</v>
+      </c>
+      <c r="O56" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="P56" s="2">
+        <v>777</v>
       </c>
       <c r="S56" s="2" t="s">
         <v>143</v>
       </c>
       <c r="T56" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A57" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E57" s="2">
+        <v>1</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="J57" s="2">
+        <v>666</v>
+      </c>
+      <c r="S57" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="T57" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G57" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="I57" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="J57" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="S57" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="T57" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A58" s="2" t="s">
         <v>147</v>
       </c>
@@ -2934,178 +2956,178 @@
         <v>21</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>260</v>
+        <v>152</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="S58" s="2" t="s">
         <v>147</v>
       </c>
       <c r="T58" s="2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A59" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E59" s="2">
-        <v>777</v>
+        <v>21</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>260</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S59" s="2" t="s">
         <v>147</v>
       </c>
       <c r="T59" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A60" s="2" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G60" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="H60" s="2" t="s">
-        <v>160</v>
+        <v>37</v>
+      </c>
+      <c r="E60" s="2">
+        <v>777</v>
       </c>
       <c r="I60" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="J60" s="2">
-        <v>1</v>
+      <c r="J60" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="S60" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="T60" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A61" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="T60" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>264</v>
+        <v>160</v>
       </c>
       <c r="I61" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="J61" s="2" t="s">
-        <v>262</v>
+      <c r="J61" s="2">
+        <v>1</v>
       </c>
       <c r="S61" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="T61" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A62" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>164</v>
+        <v>264</v>
       </c>
       <c r="I62" s="2" t="s">
         <v>143</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="S62" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="T62" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A63" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="T62" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>166</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G63" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="S63" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="T63" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A64" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="I63" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="J63" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="S63" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="T63" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="I64" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="J64" s="2">
-        <v>1</v>
+      <c r="J64" s="2" t="s">
+        <v>265</v>
       </c>
       <c r="S64" s="2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="T64" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A65" s="2" t="s">
         <v>171</v>
       </c>
@@ -3116,59 +3138,59 @@
         <v>171</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>294</v>
+        <v>172</v>
       </c>
       <c r="I65" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="J65" s="2" t="s">
-        <v>290</v>
+      <c r="J65" s="2">
+        <v>1</v>
       </c>
       <c r="S65" s="2" t="s">
         <v>171</v>
       </c>
       <c r="T65" s="2" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A66" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>175</v>
+        <v>294</v>
       </c>
       <c r="I66" s="2" t="s">
         <v>168</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
       <c r="S66" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="T66" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A67" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="T66" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
-        <v>177</v>
-      </c>
       <c r="B67" s="2" t="s">
-        <v>111</v>
+        <v>21</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>338</v>
+        <v>175</v>
       </c>
       <c r="I67" s="2" t="s">
         <v>168</v>
@@ -3176,20 +3198,14 @@
       <c r="J67" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="L67" s="2" t="s">
+      <c r="S67" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="M67" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="S67" s="2" t="s">
-        <v>177</v>
-      </c>
       <c r="T67" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A68" s="2" t="s">
         <v>177</v>
       </c>
@@ -3197,147 +3213,153 @@
         <v>111</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>306</v>
+        <v>338</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>181</v>
+        <v>265</v>
       </c>
       <c r="L68" s="2" t="s">
         <v>174</v>
       </c>
       <c r="M68" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="S68" s="2" t="s">
         <v>177</v>
       </c>
       <c r="T68" s="2" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A69" s="2" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E69" s="2">
-        <v>4</v>
+        <v>111</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>306</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="J69" s="2" t="s">
-        <v>295</v>
+        <v>181</v>
       </c>
       <c r="L69" s="2" t="s">
         <v>174</v>
       </c>
       <c r="M69" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="O69" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="S69" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="P69" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="S69" s="2" t="s">
-        <v>168</v>
-      </c>
       <c r="T69" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A70" s="2" t="s">
         <v>168</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>37</v>
+        <v>146</v>
       </c>
       <c r="E70" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I70" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="J70" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="L70" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="J70" s="2">
-        <v>666</v>
+      <c r="M70" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="O70" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="P70" s="2" t="s">
+        <v>295</v>
       </c>
       <c r="S70" s="2" t="s">
         <v>168</v>
       </c>
       <c r="T70" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A71" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E71" s="2">
+        <v>1</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="J71" s="2">
+        <v>666</v>
+      </c>
+      <c r="S71" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="T71" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A72" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G71" s="2" t="s">
+      <c r="G72" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="H71" s="2" t="s">
+      <c r="H72" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="I71" s="2" t="s">
+      <c r="I72" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="J71" s="2" t="s">
+      <c r="J72" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="L71" s="2" t="s">
+      <c r="L72" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="M71" s="2" t="s">
+      <c r="M72" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="S71" s="2" t="s">
+      <c r="S72" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="T71" s="2" t="s">
+      <c r="T72" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="H72" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="I72" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="J72" s="2">
-        <v>1</v>
-      </c>
-      <c r="S72" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="T72" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A73" s="2" t="s">
         <v>191</v>
       </c>
@@ -3348,22 +3370,22 @@
         <v>192</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="I73" s="2" t="s">
         <v>191</v>
       </c>
       <c r="J73" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S73" s="2" t="s">
         <v>192</v>
       </c>
       <c r="T73" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A74" s="2" t="s">
         <v>191</v>
       </c>
@@ -3374,71 +3396,74 @@
         <v>192</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>195</v>
+        <v>301</v>
       </c>
       <c r="I74" s="2" t="s">
         <v>191</v>
       </c>
       <c r="J74" s="2">
-        <v>888</v>
+        <v>0</v>
       </c>
       <c r="S74" s="2" t="s">
         <v>192</v>
       </c>
       <c r="T74" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A75" s="2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>302</v>
+        <v>195</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="J75" s="2">
-        <v>1</v>
+        <v>888</v>
       </c>
       <c r="S75" s="2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="T75" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A76" s="2" t="s">
         <v>197</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E76" s="2">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>302</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="J76" s="2" t="s">
-        <v>296</v>
+        <v>197</v>
+      </c>
+      <c r="J76" s="2">
+        <v>1</v>
       </c>
       <c r="S76" s="2" t="s">
         <v>198</v>
       </c>
       <c r="T76" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A77" s="2" t="s">
         <v>197</v>
       </c>
@@ -3446,57 +3471,45 @@
         <v>37</v>
       </c>
       <c r="E77" s="2">
-        <v>888</v>
+        <v>0</v>
       </c>
       <c r="I77" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="J77" s="2">
-        <v>888</v>
+      <c r="J77" s="2" t="s">
+        <v>296</v>
       </c>
       <c r="S77" s="2" t="s">
         <v>198</v>
       </c>
       <c r="T77" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A78" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E78" s="2">
+        <v>888</v>
+      </c>
+      <c r="I78" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="J78" s="2">
+        <v>888</v>
+      </c>
+      <c r="S78" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="T78" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E78" s="2">
-        <v>0</v>
-      </c>
-      <c r="I78" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="J78" s="2">
-        <v>777</v>
-      </c>
-      <c r="L78" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="M78" s="2">
-        <v>0</v>
-      </c>
-      <c r="O78" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="P78" s="2">
-        <v>777</v>
-      </c>
-      <c r="S78" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="T78" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A79" s="2" t="s">
         <v>112</v>
       </c>
@@ -3504,91 +3517,103 @@
         <v>146</v>
       </c>
       <c r="E79" s="2">
-        <v>888</v>
+        <v>0</v>
       </c>
       <c r="I79" s="2" t="s">
         <v>78</v>
       </c>
       <c r="J79" s="2">
-        <v>888</v>
+        <v>777</v>
       </c>
       <c r="L79" s="2" t="s">
         <v>98</v>
       </c>
       <c r="M79" s="2">
-        <v>888</v>
+        <v>0</v>
       </c>
       <c r="O79" s="2" t="s">
         <v>202</v>
       </c>
       <c r="P79" s="2">
-        <v>888</v>
+        <v>777</v>
       </c>
       <c r="S79" s="2" t="s">
         <v>112</v>
       </c>
       <c r="T79" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A80" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G80" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="H80" s="2" t="s">
-        <v>113</v>
+        <v>146</v>
+      </c>
+      <c r="E80" s="2">
+        <v>888</v>
       </c>
       <c r="I80" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J80" s="2">
+        <v>888</v>
+      </c>
+      <c r="L80" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="J80" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="L80" s="2" t="s">
+      <c r="M80" s="2">
+        <v>888</v>
+      </c>
+      <c r="O80" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="M80" s="2" t="s">
-        <v>205</v>
+      <c r="P80" s="2">
+        <v>888</v>
       </c>
       <c r="S80" s="2" t="s">
         <v>112</v>
       </c>
       <c r="T80" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A81" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E81" s="2">
-        <v>0</v>
+        <v>111</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="J81" s="2">
-        <v>777</v>
+        <v>98</v>
+      </c>
+      <c r="J81" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="L81" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="M81" s="2" t="s">
+        <v>205</v>
       </c>
       <c r="S81" s="2" t="s">
         <v>112</v>
       </c>
       <c r="T81" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A82" s="2" t="s">
-        <v>202</v>
+        <v>112</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>37</v>
@@ -3600,96 +3625,93 @@
         <v>207</v>
       </c>
       <c r="J82" s="2">
+        <v>777</v>
+      </c>
+      <c r="S82" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="T82" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A83" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E83" s="2">
+        <v>0</v>
+      </c>
+      <c r="I83" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="J83" s="2">
         <v>666</v>
       </c>
-      <c r="S82" s="2" t="s">
+      <c r="S83" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="T82" s="2" t="s">
+      <c r="T83" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C83" s="2">
-        <v>0</v>
-      </c>
-      <c r="D83" s="2">
-        <v>84</v>
-      </c>
-      <c r="S83" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="T83" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A84" s="2" t="s">
         <v>207</v>
       </c>
       <c r="B84" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C84" s="2">
+        <v>0</v>
+      </c>
+      <c r="D84" s="2">
+        <v>84</v>
+      </c>
+      <c r="S84" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="T84" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A85" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E84" s="2">
+      <c r="E85" s="2">
         <v>666</v>
       </c>
-      <c r="I84" s="2" t="s">
+      <c r="I85" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="J84" s="2">
+      <c r="J85" s="2">
         <v>0</v>
       </c>
-      <c r="S84" s="2" t="s">
+      <c r="S85" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="T84" s="2" t="s">
+      <c r="T85" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A86" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G85" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="H85" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="I85" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="J85" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="S85" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="T85" s="2" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
-        <v>215</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="I86" s="2" t="s">
         <v>214</v>
@@ -3698,24 +3720,24 @@
         <v>278</v>
       </c>
       <c r="S86" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="T86" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A87" s="2" t="s">
         <v>215</v>
-      </c>
-      <c r="T86" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
-        <v>217</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>280</v>
+        <v>215</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>310</v>
+        <v>279</v>
       </c>
       <c r="I87" s="2" t="s">
         <v>214</v>
@@ -3724,502 +3746,502 @@
         <v>278</v>
       </c>
       <c r="S87" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="T87" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A88" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="T87" s="2" t="s">
+      <c r="B88" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="I88" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="J88" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="S88" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="T88" s="2" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A89" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B89" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G88" s="2" t="s">
+      <c r="G89" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="H88" s="2" t="s">
+      <c r="H89" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="I88" s="2" t="s">
+      <c r="I89" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="J88" s="2" t="s">
+      <c r="J89" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="L88" s="2" t="s">
+      <c r="L89" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="M88" s="2" t="s">
+      <c r="M89" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="S88" s="2" t="s">
+      <c r="S89" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="T88" s="2" t="s">
+      <c r="T89" s="2" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A90" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B90" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E89" s="2">
+      <c r="E90" s="2">
         <v>0</v>
       </c>
-      <c r="I89" s="2" t="s">
+      <c r="I90" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="J89" s="2" t="s">
+      <c r="J90" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="L89" s="2" t="s">
+      <c r="L90" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="M89" s="2" t="s">
+      <c r="M90" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="O89" s="2" t="s">
+      <c r="O90" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="P89" s="2" t="s">
+      <c r="P90" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="S89" s="2" t="s">
+      <c r="S90" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="T89" s="2" t="s">
+      <c r="T90" s="2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A91" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E90" s="2">
-        <v>1</v>
-      </c>
-      <c r="I90" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="J90" s="2">
-        <v>666</v>
-      </c>
-      <c r="S90" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="T90" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
-        <v>217</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E91" s="2">
+        <v>1</v>
+      </c>
+      <c r="I91" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="J91" s="2">
         <v>666</v>
-      </c>
-      <c r="I91" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="J91" s="2">
-        <v>1</v>
       </c>
       <c r="S91" s="2" t="s">
         <v>219</v>
       </c>
       <c r="T91" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A92" s="2" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E92" s="2">
-        <v>1</v>
+        <v>666</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="J92" s="2">
         <v>1</v>
       </c>
       <c r="S92" s="2" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="T92" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A93" s="2" t="s">
         <v>222</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G93" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E93" s="2">
+        <v>1</v>
+      </c>
+      <c r="I93" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="H93" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="I93" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="J93" s="2">
-        <v>888</v>
+        <v>1</v>
       </c>
       <c r="S93" s="2" t="s">
         <v>223</v>
       </c>
       <c r="T93" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A94" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="H94" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="I94" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="J94" s="2">
+        <v>888</v>
+      </c>
+      <c r="S94" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="T94" s="2" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="E94" s="2">
-        <v>2</v>
-      </c>
-      <c r="I94" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="J94" s="2">
-        <v>777</v>
-      </c>
-      <c r="L94" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="M94" s="2">
-        <v>777</v>
-      </c>
-      <c r="S94" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="T94" s="2" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A95" s="2" t="s">
         <v>227</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>146</v>
+        <v>228</v>
       </c>
       <c r="E95" s="2">
         <v>2</v>
       </c>
       <c r="I95" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="J95" s="2" t="s">
-        <v>238</v>
+        <v>229</v>
+      </c>
+      <c r="J95" s="2">
+        <v>777</v>
       </c>
       <c r="L95" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="M95" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="O95" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="P95" s="2" t="s">
-        <v>238</v>
+        <v>230</v>
+      </c>
+      <c r="M95" s="2">
+        <v>777</v>
       </c>
       <c r="S95" s="2" t="s">
         <v>227</v>
       </c>
       <c r="T95" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="96" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A96" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E96" s="2">
+        <v>2</v>
+      </c>
+      <c r="I96" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="J96" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="L96" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="M96" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="O96" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="P96" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="S96" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="T96" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A97" s="2" t="s">
         <v>232</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G96" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="H96" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="I96" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="J96" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="S96" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="T96" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
-        <v>233</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="I97" s="2" t="s">
         <v>236</v>
       </c>
       <c r="J97" s="2" t="s">
-        <v>292</v>
+        <v>237</v>
       </c>
       <c r="S97" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="T97" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="98" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A98" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="T97" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
-        <v>234</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I98" s="2" t="s">
         <v>236</v>
       </c>
       <c r="J98" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="S98" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="T98" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="99" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A99" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="H99" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="I99" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="J99" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="S98" s="2" t="s">
+      <c r="S99" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="T98" s="2" t="s">
+      <c r="T99" s="2" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A100" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B100" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="E99" s="2">
-        <v>0</v>
-      </c>
-      <c r="I99" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="J99" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="L99" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="M99" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="O99" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="P99" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="S99" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="T99" s="2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="E100" s="2">
         <v>0</v>
       </c>
       <c r="I100" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J100" s="2" t="s">
         <v>298</v>
       </c>
+      <c r="L100" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="M100" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="O100" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="P100" s="2" t="s">
+        <v>298</v>
+      </c>
       <c r="S100" s="2" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="T100" s="2" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="101" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A101" s="2" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E101" s="2">
-        <v>777</v>
+        <v>0</v>
       </c>
       <c r="I101" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="J101" s="2">
-        <v>0</v>
+        <v>233</v>
+      </c>
+      <c r="J101" s="2" t="s">
+        <v>298</v>
       </c>
       <c r="S101" s="2" t="s">
         <v>233</v>
       </c>
       <c r="T101" s="2" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="102" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A102" s="2" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E102" s="2">
+        <v>777</v>
+      </c>
+      <c r="I102" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="J102" s="2">
         <v>0</v>
       </c>
-      <c r="I102" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="J102" s="2" t="s">
-        <v>298</v>
-      </c>
       <c r="S102" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="T102" s="2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="103" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A103" s="2" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E103" s="2">
-        <v>777</v>
+        <v>0</v>
       </c>
       <c r="I103" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="J103" s="2">
-        <v>0</v>
+        <v>234</v>
+      </c>
+      <c r="J103" s="2" t="s">
+        <v>298</v>
       </c>
       <c r="S103" s="2" t="s">
         <v>234</v>
       </c>
       <c r="T103" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="104" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A104" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E104" s="2">
+        <v>777</v>
+      </c>
+      <c r="I104" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="J104" s="2">
+        <v>0</v>
+      </c>
+      <c r="S104" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="T104" s="2" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G104" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="H104" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="I104" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="J104" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="L104" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="M104" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="S104" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="T104" s="2" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A105" s="2" t="s">
         <v>236</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>21</v>
+        <v>111</v>
       </c>
       <c r="G105" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="I105" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H105" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="I105" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="J105" s="2">
-        <v>0</v>
+      <c r="J105" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="L105" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="M105" s="2" t="s">
+        <v>246</v>
       </c>
       <c r="S105" s="2" t="s">
         <v>236</v>
       </c>
       <c r="T105" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="106" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A106" s="2" t="s">
         <v>236</v>
       </c>
@@ -4227,10 +4249,10 @@
         <v>21</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I106" s="2" t="s">
         <v>236</v>
@@ -4242,87 +4264,93 @@
         <v>236</v>
       </c>
       <c r="T106" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="107" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A107" s="2" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G107" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="H107" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="I107" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="J107" s="2">
+        <v>0</v>
+      </c>
+      <c r="S107" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="T107" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="108" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A108" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="H107" s="2" t="s">
+      <c r="B108" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="H108" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="I107" s="2" t="s">
+      <c r="I108" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="J107" s="2" t="s">
+      <c r="J108" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="S107" s="2" t="s">
+      <c r="S108" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="T107" s="2" t="s">
+      <c r="T108" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A109" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="B109" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="E108" s="2">
+      <c r="E109" s="2">
         <v>0</v>
       </c>
-      <c r="I108" s="2" t="s">
+      <c r="I109" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="J108" s="2">
+      <c r="J109" s="2">
         <v>777</v>
       </c>
-      <c r="L108" s="2" t="s">
+      <c r="L109" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="M108" s="2">
+      <c r="M109" s="2">
         <v>7777</v>
       </c>
-      <c r="S108" s="2" t="s">
+      <c r="S109" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="T108" s="2" t="s">
+      <c r="T109" s="2" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A109" s="2" t="s">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A110" s="2" t="s">
         <v>257</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C109" s="2">
-        <v>0</v>
-      </c>
-      <c r="D109" s="2">
-        <v>150</v>
-      </c>
-      <c r="S109" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="T109" s="2" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
-        <v>258</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>34</v>
@@ -4331,42 +4359,36 @@
         <v>0</v>
       </c>
       <c r="D110" s="2">
+        <v>150</v>
+      </c>
+      <c r="S110" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="T110" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="111" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A111" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C111" s="2">
+        <v>0</v>
+      </c>
+      <c r="D111" s="2">
         <v>100</v>
       </c>
-      <c r="S110" s="2" t="s">
+      <c r="S111" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="T110" s="2" t="s">
+      <c r="T111" s="2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G111" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="H111" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="I111" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J111" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S111" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="T111" s="2" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A112" s="2" t="s">
         <v>342</v>
       </c>
@@ -4377,7 +4399,7 @@
         <v>342</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I112" s="2" t="s">
         <v>25</v>
@@ -4389,10 +4411,10 @@
         <v>342</v>
       </c>
       <c r="T112" s="2" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="113" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A113" s="2" t="s">
         <v>342</v>
       </c>
@@ -4403,7 +4425,7 @@
         <v>342</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="I113" s="2" t="s">
         <v>25</v>
@@ -4415,11 +4437,37 @@
         <v>342</v>
       </c>
       <c r="T113" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="114" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A114" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G114" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="H114" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="I114" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J114" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="S114" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="T114" s="2" t="s">
         <v>348</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T110" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:T111" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4432,7 +4480,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4445,7 +4493,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>